<commit_message>
Updated milestones and other activities
</commit_message>
<xml_diff>
--- a/SaintLukeConfirmationRetreatRoadmap.xlsx
+++ b/SaintLukeConfirmationRetreatRoadmap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marceljemio/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17C9528-13A4-DD44-8990-C3DBEB918022}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1287078E-EA9A-9440-99A8-09DDA82598D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-160" yWindow="460" windowWidth="28800" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
   <si>
     <t>Meet to review ideas for Faith Experience</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Meet with Confirmandi about the Play</t>
   </si>
   <si>
-    <t>Setup Rehearsals</t>
-  </si>
-  <si>
     <t>Order YouCat books</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>Expand Flaherty Hall access for more rehearsals/setup times</t>
   </si>
   <si>
-    <t>Deliver the faith sessions</t>
-  </si>
-  <si>
     <t>Core Team Meeing</t>
   </si>
   <si>
@@ -76,9 +70,6 @@
     <t>Finalize the song list</t>
   </si>
   <si>
-    <t>Finalize layout of Flaherty Hall</t>
-  </si>
-  <si>
     <t>Update the script</t>
   </si>
   <si>
@@ -91,18 +82,12 @@
     <t>Don Bosco Volunteer Training</t>
   </si>
   <si>
-    <t>Meet with Confirmandi about the Play.  Email update to Parents</t>
-  </si>
-  <si>
     <t>Order Confirmation Retreat t-shirts</t>
   </si>
   <si>
     <t>Arrange for proper layout of Hall and Narthex</t>
   </si>
   <si>
-    <t>Ensure smooth operation of Confirmatin Retreat</t>
-  </si>
-  <si>
     <t>Review volunteer, parent, and student feedback from last year</t>
   </si>
   <si>
@@ -124,33 +109,15 @@
     <t>Saving Grace Play (Play)</t>
   </si>
   <si>
-    <t>Retreat update sent to parents</t>
-  </si>
-  <si>
-    <t>Core Team Meeing.  Update to parents.</t>
-  </si>
-  <si>
-    <t>Core Team Meeing.  Update to parents and volunteer signup</t>
-  </si>
-  <si>
-    <t>Core Team Meeing.  Update to parents</t>
-  </si>
-  <si>
     <t>Confirmation Mass Rehearsal and Mass</t>
   </si>
   <si>
-    <t>Take video and pictures of events</t>
-  </si>
-  <si>
     <t>Compile video for after Confirmation mass</t>
   </si>
   <si>
     <t>Identify props</t>
   </si>
   <si>
-    <t>Finalize props</t>
-  </si>
-  <si>
     <t>Add roles in Act 3 and work out skits for songs</t>
   </si>
   <si>
@@ -160,9 +127,6 @@
     <t>Finalize sessions and confirm speakers, rooms, and other needs</t>
   </si>
   <si>
-    <t>Secure printer for check-in and print materials for FX, RS, and Play</t>
-  </si>
-  <si>
     <t>Finalize the script and song skits</t>
   </si>
   <si>
@@ -184,18 +148,12 @@
     <t>Communicate with Volunteers</t>
   </si>
   <si>
-    <t>Identify videographer(s), photographer(s)</t>
-  </si>
-  <si>
     <t>Prepare material and handouts</t>
   </si>
   <si>
     <t>Measure the students in the PSR or Saint Luke School class for robes.</t>
   </si>
   <si>
-    <t>Version 20181126</t>
-  </si>
-  <si>
     <t>Prepare parent session</t>
   </si>
   <si>
@@ -206,6 +164,57 @@
   </si>
   <si>
     <t>Order Confirmandi gifts (wristbands, stickers, phone covers, hoodies, etc)</t>
+  </si>
+  <si>
+    <t>Parent meeting</t>
+  </si>
+  <si>
+    <t>Core Team Meeing.  Email update to parents.</t>
+  </si>
+  <si>
+    <t>Core Team Meeing.  Parent meeting/Email and Retreat volunteer signup</t>
+  </si>
+  <si>
+    <t>Version 20181129</t>
+  </si>
+  <si>
+    <t>Finalize prop needs</t>
+  </si>
+  <si>
+    <t>Deliver the faith experience sessions</t>
+  </si>
+  <si>
+    <t>Communicate with Volunteers before the Retreat for final preparation</t>
+  </si>
+  <si>
+    <t>Conduct feedback survey of volunteers, parents, and students.</t>
+  </si>
+  <si>
+    <t>Analyze feedback and prepare for next year's improvements.</t>
+  </si>
+  <si>
+    <t>Setup Final Rehearsals within the 2-weeks before the Retreat.</t>
+  </si>
+  <si>
+    <t>Integrate Flaherty Hall sound/light into stage management</t>
+  </si>
+  <si>
+    <t>Prepare for sensory-friendly explanation to audience before the play.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meet with Confirmandi about the Play.  </t>
+  </si>
+  <si>
+    <t>Retreat Milestones</t>
+  </si>
+  <si>
+    <t>Deliver and ensure smooth operation of Confirmatin Retreat</t>
+  </si>
+  <si>
+    <t>Finalize layout of Flaherty Hall (to include sensory-friendly changes)</t>
+  </si>
+  <si>
+    <t>Secure printer for check-in and print materials for FX, RS, and Play teams</t>
   </si>
 </sst>
 </file>
@@ -215,7 +224,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -223,38 +232,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color indexed="8"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color indexed="8"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color indexed="12"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color indexed="8"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color indexed="8"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -267,7 +244,39 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="16"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color indexed="12"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color indexed="8"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -489,14 +498,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -504,20 +522,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1711,10 +1720,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV18"/>
+  <dimension ref="A1:IV22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="88" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1725,8 +1734,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="29" t="s">
-        <v>57</v>
+      <c r="A1" s="25" t="s">
+        <v>51</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="18"/>
@@ -1742,7 +1751,7 @@
     </row>
     <row r="2" spans="1:256" ht="48" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="18"/>
@@ -1757,8 +1766,8 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:256" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>51</v>
+      <c r="A3" s="26" t="s">
+        <v>39</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="19"/>
@@ -2052,34 +2061,38 @@
       <c r="IU4" s="10"/>
       <c r="IV4" s="10"/>
     </row>
-    <row r="5" spans="1:256" s="14" customFormat="1" ht="58" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:256" s="14" customFormat="1" ht="96" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="16" t="s">
+        <v>61</v>
+      </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
-      <c r="D5" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>38</v>
+      <c r="D5" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>29</v>
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
@@ -2326,39 +2339,19 @@
       <c r="IU5" s="13"/>
       <c r="IV5" s="13"/>
     </row>
-    <row r="6" spans="1:256" s="14" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>40</v>
-      </c>
+    <row r="6" spans="1:256" s="24" customFormat="1" ht="23" x14ac:dyDescent="0.15">
+      <c r="A6" s="16"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
@@ -2604,25 +2597,39 @@
       <c r="IU6" s="13"/>
       <c r="IV6" s="13"/>
     </row>
-    <row r="7" spans="1:256" s="14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="27"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+    <row r="7" spans="1:256" s="14" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>0</v>
+      </c>
       <c r="F7" s="20" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
@@ -2868,19 +2875,27 @@
       <c r="IU7" s="13"/>
       <c r="IV7" s="13"/>
     </row>
-    <row r="8" spans="1:256" s="14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="27"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
+    <row r="8" spans="1:256" s="14" customFormat="1" ht="57" x14ac:dyDescent="0.15">
+      <c r="A8" s="30"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="20"/>
       <c r="K8" s="20"/>
-      <c r="L8" s="21"/>
+      <c r="L8" s="20" t="s">
+        <v>56</v>
+      </c>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
@@ -3127,18 +3142,18 @@
       <c r="IV8" s="13"/>
     </row>
     <row r="9" spans="1:256" s="14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="15"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="21"/>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
@@ -3384,405 +3399,385 @@
       <c r="IU9" s="13"/>
       <c r="IV9" s="13"/>
     </row>
-    <row r="10" spans="1:256" ht="57" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="20" t="s">
+    <row r="10" spans="1:256" s="14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="15"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="13"/>
+      <c r="AH10" s="13"/>
+      <c r="AI10" s="13"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="13"/>
+      <c r="AM10" s="13"/>
+      <c r="AN10" s="13"/>
+      <c r="AO10" s="13"/>
+      <c r="AP10" s="13"/>
+      <c r="AQ10" s="13"/>
+      <c r="AR10" s="13"/>
+      <c r="AS10" s="13"/>
+      <c r="AT10" s="13"/>
+      <c r="AU10" s="13"/>
+      <c r="AV10" s="13"/>
+      <c r="AW10" s="13"/>
+      <c r="AX10" s="13"/>
+      <c r="AY10" s="13"/>
+      <c r="AZ10" s="13"/>
+      <c r="BA10" s="13"/>
+      <c r="BB10" s="13"/>
+      <c r="BC10" s="13"/>
+      <c r="BD10" s="13"/>
+      <c r="BE10" s="13"/>
+      <c r="BF10" s="13"/>
+      <c r="BG10" s="13"/>
+      <c r="BH10" s="13"/>
+      <c r="BI10" s="13"/>
+      <c r="BJ10" s="13"/>
+      <c r="BK10" s="13"/>
+      <c r="BL10" s="13"/>
+      <c r="BM10" s="13"/>
+      <c r="BN10" s="13"/>
+      <c r="BO10" s="13"/>
+      <c r="BP10" s="13"/>
+      <c r="BQ10" s="13"/>
+      <c r="BR10" s="13"/>
+      <c r="BS10" s="13"/>
+      <c r="BT10" s="13"/>
+      <c r="BU10" s="13"/>
+      <c r="BV10" s="13"/>
+      <c r="BW10" s="13"/>
+      <c r="BX10" s="13"/>
+      <c r="BY10" s="13"/>
+      <c r="BZ10" s="13"/>
+      <c r="CA10" s="13"/>
+      <c r="CB10" s="13"/>
+      <c r="CC10" s="13"/>
+      <c r="CD10" s="13"/>
+      <c r="CE10" s="13"/>
+      <c r="CF10" s="13"/>
+      <c r="CG10" s="13"/>
+      <c r="CH10" s="13"/>
+      <c r="CI10" s="13"/>
+      <c r="CJ10" s="13"/>
+      <c r="CK10" s="13"/>
+      <c r="CL10" s="13"/>
+      <c r="CM10" s="13"/>
+      <c r="CN10" s="13"/>
+      <c r="CO10" s="13"/>
+      <c r="CP10" s="13"/>
+      <c r="CQ10" s="13"/>
+      <c r="CR10" s="13"/>
+      <c r="CS10" s="13"/>
+      <c r="CT10" s="13"/>
+      <c r="CU10" s="13"/>
+      <c r="CV10" s="13"/>
+      <c r="CW10" s="13"/>
+      <c r="CX10" s="13"/>
+      <c r="CY10" s="13"/>
+      <c r="CZ10" s="13"/>
+      <c r="DA10" s="13"/>
+      <c r="DB10" s="13"/>
+      <c r="DC10" s="13"/>
+      <c r="DD10" s="13"/>
+      <c r="DE10" s="13"/>
+      <c r="DF10" s="13"/>
+      <c r="DG10" s="13"/>
+      <c r="DH10" s="13"/>
+      <c r="DI10" s="13"/>
+      <c r="DJ10" s="13"/>
+      <c r="DK10" s="13"/>
+      <c r="DL10" s="13"/>
+      <c r="DM10" s="13"/>
+      <c r="DN10" s="13"/>
+      <c r="DO10" s="13"/>
+      <c r="DP10" s="13"/>
+      <c r="DQ10" s="13"/>
+      <c r="DR10" s="13"/>
+      <c r="DS10" s="13"/>
+      <c r="DT10" s="13"/>
+      <c r="DU10" s="13"/>
+      <c r="DV10" s="13"/>
+      <c r="DW10" s="13"/>
+      <c r="DX10" s="13"/>
+      <c r="DY10" s="13"/>
+      <c r="DZ10" s="13"/>
+      <c r="EA10" s="13"/>
+      <c r="EB10" s="13"/>
+      <c r="EC10" s="13"/>
+      <c r="ED10" s="13"/>
+      <c r="EE10" s="13"/>
+      <c r="EF10" s="13"/>
+      <c r="EG10" s="13"/>
+      <c r="EH10" s="13"/>
+      <c r="EI10" s="13"/>
+      <c r="EJ10" s="13"/>
+      <c r="EK10" s="13"/>
+      <c r="EL10" s="13"/>
+      <c r="EM10" s="13"/>
+      <c r="EN10" s="13"/>
+      <c r="EO10" s="13"/>
+      <c r="EP10" s="13"/>
+      <c r="EQ10" s="13"/>
+      <c r="ER10" s="13"/>
+      <c r="ES10" s="13"/>
+      <c r="ET10" s="13"/>
+      <c r="EU10" s="13"/>
+      <c r="EV10" s="13"/>
+      <c r="EW10" s="13"/>
+      <c r="EX10" s="13"/>
+      <c r="EY10" s="13"/>
+      <c r="EZ10" s="13"/>
+      <c r="FA10" s="13"/>
+      <c r="FB10" s="13"/>
+      <c r="FC10" s="13"/>
+      <c r="FD10" s="13"/>
+      <c r="FE10" s="13"/>
+      <c r="FF10" s="13"/>
+      <c r="FG10" s="13"/>
+      <c r="FH10" s="13"/>
+      <c r="FI10" s="13"/>
+      <c r="FJ10" s="13"/>
+      <c r="FK10" s="13"/>
+      <c r="FL10" s="13"/>
+      <c r="FM10" s="13"/>
+      <c r="FN10" s="13"/>
+      <c r="FO10" s="13"/>
+      <c r="FP10" s="13"/>
+      <c r="FQ10" s="13"/>
+      <c r="FR10" s="13"/>
+      <c r="FS10" s="13"/>
+      <c r="FT10" s="13"/>
+      <c r="FU10" s="13"/>
+      <c r="FV10" s="13"/>
+      <c r="FW10" s="13"/>
+      <c r="FX10" s="13"/>
+      <c r="FY10" s="13"/>
+      <c r="FZ10" s="13"/>
+      <c r="GA10" s="13"/>
+      <c r="GB10" s="13"/>
+      <c r="GC10" s="13"/>
+      <c r="GD10" s="13"/>
+      <c r="GE10" s="13"/>
+      <c r="GF10" s="13"/>
+      <c r="GG10" s="13"/>
+      <c r="GH10" s="13"/>
+      <c r="GI10" s="13"/>
+      <c r="GJ10" s="13"/>
+      <c r="GK10" s="13"/>
+      <c r="GL10" s="13"/>
+      <c r="GM10" s="13"/>
+      <c r="GN10" s="13"/>
+      <c r="GO10" s="13"/>
+      <c r="GP10" s="13"/>
+      <c r="GQ10" s="13"/>
+      <c r="GR10" s="13"/>
+      <c r="GS10" s="13"/>
+      <c r="GT10" s="13"/>
+      <c r="GU10" s="13"/>
+      <c r="GV10" s="13"/>
+      <c r="GW10" s="13"/>
+      <c r="GX10" s="13"/>
+      <c r="GY10" s="13"/>
+      <c r="GZ10" s="13"/>
+      <c r="HA10" s="13"/>
+      <c r="HB10" s="13"/>
+      <c r="HC10" s="13"/>
+      <c r="HD10" s="13"/>
+      <c r="HE10" s="13"/>
+      <c r="HF10" s="13"/>
+      <c r="HG10" s="13"/>
+      <c r="HH10" s="13"/>
+      <c r="HI10" s="13"/>
+      <c r="HJ10" s="13"/>
+      <c r="HK10" s="13"/>
+      <c r="HL10" s="13"/>
+      <c r="HM10" s="13"/>
+      <c r="HN10" s="13"/>
+      <c r="HO10" s="13"/>
+      <c r="HP10" s="13"/>
+      <c r="HQ10" s="13"/>
+      <c r="HR10" s="13"/>
+      <c r="HS10" s="13"/>
+      <c r="HT10" s="13"/>
+      <c r="HU10" s="13"/>
+      <c r="HV10" s="13"/>
+      <c r="HW10" s="13"/>
+      <c r="HX10" s="13"/>
+      <c r="HY10" s="13"/>
+      <c r="HZ10" s="13"/>
+      <c r="IA10" s="13"/>
+      <c r="IB10" s="13"/>
+      <c r="IC10" s="13"/>
+      <c r="ID10" s="13"/>
+      <c r="IE10" s="13"/>
+      <c r="IF10" s="13"/>
+      <c r="IG10" s="13"/>
+      <c r="IH10" s="13"/>
+      <c r="II10" s="13"/>
+      <c r="IJ10" s="13"/>
+      <c r="IK10" s="13"/>
+      <c r="IL10" s="13"/>
+      <c r="IM10" s="13"/>
+      <c r="IN10" s="13"/>
+      <c r="IO10" s="13"/>
+      <c r="IP10" s="13"/>
+      <c r="IQ10" s="13"/>
+      <c r="IR10" s="13"/>
+      <c r="IS10" s="13"/>
+      <c r="IT10" s="13"/>
+      <c r="IU10" s="13"/>
+      <c r="IV10" s="13"/>
+    </row>
+    <row r="11" spans="1:256" ht="57" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="D11" s="20"/>
+      <c r="E11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" s="20"/>
-    </row>
-    <row r="11" spans="1:256" ht="76" x14ac:dyDescent="0.15">
-      <c r="A11" s="27"/>
-      <c r="B11" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="20"/>
+      <c r="K11" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:256" ht="76" x14ac:dyDescent="0.15">
-      <c r="A12" s="27"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="20" t="s">
+      <c r="F12" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="L12" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="J12" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="L12" s="20"/>
     </row>
-    <row r="13" spans="1:256" ht="57" x14ac:dyDescent="0.15">
-      <c r="A13" s="25"/>
+    <row r="13" spans="1:256" ht="76" x14ac:dyDescent="0.15">
+      <c r="A13" s="30"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="28" t="s">
-        <v>60</v>
+      <c r="G13" s="27"/>
+      <c r="H13" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" s="21"/>
+        <v>43</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="L13" s="20"/>
     </row>
-    <row r="14" spans="1:256" s="14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="16"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="13"/>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="13"/>
-      <c r="AD14" s="13"/>
-      <c r="AE14" s="13"/>
-      <c r="AF14" s="13"/>
-      <c r="AG14" s="13"/>
-      <c r="AH14" s="13"/>
-      <c r="AI14" s="13"/>
-      <c r="AJ14" s="13"/>
-      <c r="AK14" s="13"/>
-      <c r="AL14" s="13"/>
-      <c r="AM14" s="13"/>
-      <c r="AN14" s="13"/>
-      <c r="AO14" s="13"/>
-      <c r="AP14" s="13"/>
-      <c r="AQ14" s="13"/>
-      <c r="AR14" s="13"/>
-      <c r="AS14" s="13"/>
-      <c r="AT14" s="13"/>
-      <c r="AU14" s="13"/>
-      <c r="AV14" s="13"/>
-      <c r="AW14" s="13"/>
-      <c r="AX14" s="13"/>
-      <c r="AY14" s="13"/>
-      <c r="AZ14" s="13"/>
-      <c r="BA14" s="13"/>
-      <c r="BB14" s="13"/>
-      <c r="BC14" s="13"/>
-      <c r="BD14" s="13"/>
-      <c r="BE14" s="13"/>
-      <c r="BF14" s="13"/>
-      <c r="BG14" s="13"/>
-      <c r="BH14" s="13"/>
-      <c r="BI14" s="13"/>
-      <c r="BJ14" s="13"/>
-      <c r="BK14" s="13"/>
-      <c r="BL14" s="13"/>
-      <c r="BM14" s="13"/>
-      <c r="BN14" s="13"/>
-      <c r="BO14" s="13"/>
-      <c r="BP14" s="13"/>
-      <c r="BQ14" s="13"/>
-      <c r="BR14" s="13"/>
-      <c r="BS14" s="13"/>
-      <c r="BT14" s="13"/>
-      <c r="BU14" s="13"/>
-      <c r="BV14" s="13"/>
-      <c r="BW14" s="13"/>
-      <c r="BX14" s="13"/>
-      <c r="BY14" s="13"/>
-      <c r="BZ14" s="13"/>
-      <c r="CA14" s="13"/>
-      <c r="CB14" s="13"/>
-      <c r="CC14" s="13"/>
-      <c r="CD14" s="13"/>
-      <c r="CE14" s="13"/>
-      <c r="CF14" s="13"/>
-      <c r="CG14" s="13"/>
-      <c r="CH14" s="13"/>
-      <c r="CI14" s="13"/>
-      <c r="CJ14" s="13"/>
-      <c r="CK14" s="13"/>
-      <c r="CL14" s="13"/>
-      <c r="CM14" s="13"/>
-      <c r="CN14" s="13"/>
-      <c r="CO14" s="13"/>
-      <c r="CP14" s="13"/>
-      <c r="CQ14" s="13"/>
-      <c r="CR14" s="13"/>
-      <c r="CS14" s="13"/>
-      <c r="CT14" s="13"/>
-      <c r="CU14" s="13"/>
-      <c r="CV14" s="13"/>
-      <c r="CW14" s="13"/>
-      <c r="CX14" s="13"/>
-      <c r="CY14" s="13"/>
-      <c r="CZ14" s="13"/>
-      <c r="DA14" s="13"/>
-      <c r="DB14" s="13"/>
-      <c r="DC14" s="13"/>
-      <c r="DD14" s="13"/>
-      <c r="DE14" s="13"/>
-      <c r="DF14" s="13"/>
-      <c r="DG14" s="13"/>
-      <c r="DH14" s="13"/>
-      <c r="DI14" s="13"/>
-      <c r="DJ14" s="13"/>
-      <c r="DK14" s="13"/>
-      <c r="DL14" s="13"/>
-      <c r="DM14" s="13"/>
-      <c r="DN14" s="13"/>
-      <c r="DO14" s="13"/>
-      <c r="DP14" s="13"/>
-      <c r="DQ14" s="13"/>
-      <c r="DR14" s="13"/>
-      <c r="DS14" s="13"/>
-      <c r="DT14" s="13"/>
-      <c r="DU14" s="13"/>
-      <c r="DV14" s="13"/>
-      <c r="DW14" s="13"/>
-      <c r="DX14" s="13"/>
-      <c r="DY14" s="13"/>
-      <c r="DZ14" s="13"/>
-      <c r="EA14" s="13"/>
-      <c r="EB14" s="13"/>
-      <c r="EC14" s="13"/>
-      <c r="ED14" s="13"/>
-      <c r="EE14" s="13"/>
-      <c r="EF14" s="13"/>
-      <c r="EG14" s="13"/>
-      <c r="EH14" s="13"/>
-      <c r="EI14" s="13"/>
-      <c r="EJ14" s="13"/>
-      <c r="EK14" s="13"/>
-      <c r="EL14" s="13"/>
-      <c r="EM14" s="13"/>
-      <c r="EN14" s="13"/>
-      <c r="EO14" s="13"/>
-      <c r="EP14" s="13"/>
-      <c r="EQ14" s="13"/>
-      <c r="ER14" s="13"/>
-      <c r="ES14" s="13"/>
-      <c r="ET14" s="13"/>
-      <c r="EU14" s="13"/>
-      <c r="EV14" s="13"/>
-      <c r="EW14" s="13"/>
-      <c r="EX14" s="13"/>
-      <c r="EY14" s="13"/>
-      <c r="EZ14" s="13"/>
-      <c r="FA14" s="13"/>
-      <c r="FB14" s="13"/>
-      <c r="FC14" s="13"/>
-      <c r="FD14" s="13"/>
-      <c r="FE14" s="13"/>
-      <c r="FF14" s="13"/>
-      <c r="FG14" s="13"/>
-      <c r="FH14" s="13"/>
-      <c r="FI14" s="13"/>
-      <c r="FJ14" s="13"/>
-      <c r="FK14" s="13"/>
-      <c r="FL14" s="13"/>
-      <c r="FM14" s="13"/>
-      <c r="FN14" s="13"/>
-      <c r="FO14" s="13"/>
-      <c r="FP14" s="13"/>
-      <c r="FQ14" s="13"/>
-      <c r="FR14" s="13"/>
-      <c r="FS14" s="13"/>
-      <c r="FT14" s="13"/>
-      <c r="FU14" s="13"/>
-      <c r="FV14" s="13"/>
-      <c r="FW14" s="13"/>
-      <c r="FX14" s="13"/>
-      <c r="FY14" s="13"/>
-      <c r="FZ14" s="13"/>
-      <c r="GA14" s="13"/>
-      <c r="GB14" s="13"/>
-      <c r="GC14" s="13"/>
-      <c r="GD14" s="13"/>
-      <c r="GE14" s="13"/>
-      <c r="GF14" s="13"/>
-      <c r="GG14" s="13"/>
-      <c r="GH14" s="13"/>
-      <c r="GI14" s="13"/>
-      <c r="GJ14" s="13"/>
-      <c r="GK14" s="13"/>
-      <c r="GL14" s="13"/>
-      <c r="GM14" s="13"/>
-      <c r="GN14" s="13"/>
-      <c r="GO14" s="13"/>
-      <c r="GP14" s="13"/>
-      <c r="GQ14" s="13"/>
-      <c r="GR14" s="13"/>
-      <c r="GS14" s="13"/>
-      <c r="GT14" s="13"/>
-      <c r="GU14" s="13"/>
-      <c r="GV14" s="13"/>
-      <c r="GW14" s="13"/>
-      <c r="GX14" s="13"/>
-      <c r="GY14" s="13"/>
-      <c r="GZ14" s="13"/>
-      <c r="HA14" s="13"/>
-      <c r="HB14" s="13"/>
-      <c r="HC14" s="13"/>
-      <c r="HD14" s="13"/>
-      <c r="HE14" s="13"/>
-      <c r="HF14" s="13"/>
-      <c r="HG14" s="13"/>
-      <c r="HH14" s="13"/>
-      <c r="HI14" s="13"/>
-      <c r="HJ14" s="13"/>
-      <c r="HK14" s="13"/>
-      <c r="HL14" s="13"/>
-      <c r="HM14" s="13"/>
-      <c r="HN14" s="13"/>
-      <c r="HO14" s="13"/>
-      <c r="HP14" s="13"/>
-      <c r="HQ14" s="13"/>
-      <c r="HR14" s="13"/>
-      <c r="HS14" s="13"/>
-      <c r="HT14" s="13"/>
-      <c r="HU14" s="13"/>
-      <c r="HV14" s="13"/>
-      <c r="HW14" s="13"/>
-      <c r="HX14" s="13"/>
-      <c r="HY14" s="13"/>
-      <c r="HZ14" s="13"/>
-      <c r="IA14" s="13"/>
-      <c r="IB14" s="13"/>
-      <c r="IC14" s="13"/>
-      <c r="ID14" s="13"/>
-      <c r="IE14" s="13"/>
-      <c r="IF14" s="13"/>
-      <c r="IG14" s="13"/>
-      <c r="IH14" s="13"/>
-      <c r="II14" s="13"/>
-      <c r="IJ14" s="13"/>
-      <c r="IK14" s="13"/>
-      <c r="IL14" s="13"/>
-      <c r="IM14" s="13"/>
-      <c r="IN14" s="13"/>
-      <c r="IO14" s="13"/>
-      <c r="IP14" s="13"/>
-      <c r="IQ14" s="13"/>
-      <c r="IR14" s="13"/>
-      <c r="IS14" s="13"/>
-      <c r="IT14" s="13"/>
-      <c r="IU14" s="13"/>
-      <c r="IV14" s="13"/>
+    <row r="14" spans="1:256" ht="38" x14ac:dyDescent="0.15">
+      <c r="A14" s="23"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" s="21"/>
+      <c r="L14" s="20"/>
     </row>
-    <row r="15" spans="1:256" s="14" customFormat="1" ht="57" x14ac:dyDescent="0.15">
-      <c r="A15" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="L15" s="20" t="s">
-        <v>40</v>
-      </c>
+    <row r="15" spans="1:256" s="14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="16"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
@@ -4028,37 +4023,43 @@
       <c r="IU15" s="13"/>
       <c r="IV15" s="13"/>
     </row>
-    <row r="16" spans="1:256" s="14" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="27"/>
+    <row r="16" spans="1:256" s="14" customFormat="1" ht="76" x14ac:dyDescent="0.15">
+      <c r="A16" s="29" t="s">
+        <v>28</v>
+      </c>
       <c r="B16" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
@@ -4304,31 +4305,39 @@
       <c r="IU16" s="13"/>
       <c r="IV16" s="13"/>
     </row>
-    <row r="17" spans="1:256" s="14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="27"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
+    <row r="17" spans="1:256" s="14" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="30"/>
+      <c r="B17" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>4</v>
+      </c>
       <c r="K17" s="20"/>
-      <c r="L17" s="21"/>
+      <c r="L17" s="20" t="s">
+        <v>56</v>
+      </c>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
@@ -4574,25 +4583,31 @@
       <c r="IU17" s="13"/>
       <c r="IV17" s="13"/>
     </row>
-    <row r="18" spans="1:256" s="25" customFormat="1" ht="57" x14ac:dyDescent="0.15">
-      <c r="A18" s="16"/>
+    <row r="18" spans="1:256" s="14" customFormat="1" ht="57" x14ac:dyDescent="0.15">
+      <c r="A18" s="30"/>
       <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
+      <c r="C18" s="20" t="s">
+        <v>3</v>
+      </c>
       <c r="D18" s="20" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="H18" s="20"/>
+        <v>15</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>35</v>
+      </c>
       <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
+      <c r="J18" s="20" t="s">
+        <v>58</v>
+      </c>
       <c r="K18" s="20"/>
       <c r="L18" s="21"/>
       <c r="M18" s="13"/>
@@ -4840,11 +4855,316 @@
       <c r="IU18" s="13"/>
       <c r="IV18" s="13"/>
     </row>
+    <row r="19" spans="1:256" s="23" customFormat="1" ht="76" x14ac:dyDescent="0.15">
+      <c r="A19" s="16"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="K19" s="20"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="13"/>
+      <c r="AC19" s="13"/>
+      <c r="AD19" s="13"/>
+      <c r="AE19" s="13"/>
+      <c r="AF19" s="13"/>
+      <c r="AG19" s="13"/>
+      <c r="AH19" s="13"/>
+      <c r="AI19" s="13"/>
+      <c r="AJ19" s="13"/>
+      <c r="AK19" s="13"/>
+      <c r="AL19" s="13"/>
+      <c r="AM19" s="13"/>
+      <c r="AN19" s="13"/>
+      <c r="AO19" s="13"/>
+      <c r="AP19" s="13"/>
+      <c r="AQ19" s="13"/>
+      <c r="AR19" s="13"/>
+      <c r="AS19" s="13"/>
+      <c r="AT19" s="13"/>
+      <c r="AU19" s="13"/>
+      <c r="AV19" s="13"/>
+      <c r="AW19" s="13"/>
+      <c r="AX19" s="13"/>
+      <c r="AY19" s="13"/>
+      <c r="AZ19" s="13"/>
+      <c r="BA19" s="13"/>
+      <c r="BB19" s="13"/>
+      <c r="BC19" s="13"/>
+      <c r="BD19" s="13"/>
+      <c r="BE19" s="13"/>
+      <c r="BF19" s="13"/>
+      <c r="BG19" s="13"/>
+      <c r="BH19" s="13"/>
+      <c r="BI19" s="13"/>
+      <c r="BJ19" s="13"/>
+      <c r="BK19" s="13"/>
+      <c r="BL19" s="13"/>
+      <c r="BM19" s="13"/>
+      <c r="BN19" s="13"/>
+      <c r="BO19" s="13"/>
+      <c r="BP19" s="13"/>
+      <c r="BQ19" s="13"/>
+      <c r="BR19" s="13"/>
+      <c r="BS19" s="13"/>
+      <c r="BT19" s="13"/>
+      <c r="BU19" s="13"/>
+      <c r="BV19" s="13"/>
+      <c r="BW19" s="13"/>
+      <c r="BX19" s="13"/>
+      <c r="BY19" s="13"/>
+      <c r="BZ19" s="13"/>
+      <c r="CA19" s="13"/>
+      <c r="CB19" s="13"/>
+      <c r="CC19" s="13"/>
+      <c r="CD19" s="13"/>
+      <c r="CE19" s="13"/>
+      <c r="CF19" s="13"/>
+      <c r="CG19" s="13"/>
+      <c r="CH19" s="13"/>
+      <c r="CI19" s="13"/>
+      <c r="CJ19" s="13"/>
+      <c r="CK19" s="13"/>
+      <c r="CL19" s="13"/>
+      <c r="CM19" s="13"/>
+      <c r="CN19" s="13"/>
+      <c r="CO19" s="13"/>
+      <c r="CP19" s="13"/>
+      <c r="CQ19" s="13"/>
+      <c r="CR19" s="13"/>
+      <c r="CS19" s="13"/>
+      <c r="CT19" s="13"/>
+      <c r="CU19" s="13"/>
+      <c r="CV19" s="13"/>
+      <c r="CW19" s="13"/>
+      <c r="CX19" s="13"/>
+      <c r="CY19" s="13"/>
+      <c r="CZ19" s="13"/>
+      <c r="DA19" s="13"/>
+      <c r="DB19" s="13"/>
+      <c r="DC19" s="13"/>
+      <c r="DD19" s="13"/>
+      <c r="DE19" s="13"/>
+      <c r="DF19" s="13"/>
+      <c r="DG19" s="13"/>
+      <c r="DH19" s="13"/>
+      <c r="DI19" s="13"/>
+      <c r="DJ19" s="13"/>
+      <c r="DK19" s="13"/>
+      <c r="DL19" s="13"/>
+      <c r="DM19" s="13"/>
+      <c r="DN19" s="13"/>
+      <c r="DO19" s="13"/>
+      <c r="DP19" s="13"/>
+      <c r="DQ19" s="13"/>
+      <c r="DR19" s="13"/>
+      <c r="DS19" s="13"/>
+      <c r="DT19" s="13"/>
+      <c r="DU19" s="13"/>
+      <c r="DV19" s="13"/>
+      <c r="DW19" s="13"/>
+      <c r="DX19" s="13"/>
+      <c r="DY19" s="13"/>
+      <c r="DZ19" s="13"/>
+      <c r="EA19" s="13"/>
+      <c r="EB19" s="13"/>
+      <c r="EC19" s="13"/>
+      <c r="ED19" s="13"/>
+      <c r="EE19" s="13"/>
+      <c r="EF19" s="13"/>
+      <c r="EG19" s="13"/>
+      <c r="EH19" s="13"/>
+      <c r="EI19" s="13"/>
+      <c r="EJ19" s="13"/>
+      <c r="EK19" s="13"/>
+      <c r="EL19" s="13"/>
+      <c r="EM19" s="13"/>
+      <c r="EN19" s="13"/>
+      <c r="EO19" s="13"/>
+      <c r="EP19" s="13"/>
+      <c r="EQ19" s="13"/>
+      <c r="ER19" s="13"/>
+      <c r="ES19" s="13"/>
+      <c r="ET19" s="13"/>
+      <c r="EU19" s="13"/>
+      <c r="EV19" s="13"/>
+      <c r="EW19" s="13"/>
+      <c r="EX19" s="13"/>
+      <c r="EY19" s="13"/>
+      <c r="EZ19" s="13"/>
+      <c r="FA19" s="13"/>
+      <c r="FB19" s="13"/>
+      <c r="FC19" s="13"/>
+      <c r="FD19" s="13"/>
+      <c r="FE19" s="13"/>
+      <c r="FF19" s="13"/>
+      <c r="FG19" s="13"/>
+      <c r="FH19" s="13"/>
+      <c r="FI19" s="13"/>
+      <c r="FJ19" s="13"/>
+      <c r="FK19" s="13"/>
+      <c r="FL19" s="13"/>
+      <c r="FM19" s="13"/>
+      <c r="FN19" s="13"/>
+      <c r="FO19" s="13"/>
+      <c r="FP19" s="13"/>
+      <c r="FQ19" s="13"/>
+      <c r="FR19" s="13"/>
+      <c r="FS19" s="13"/>
+      <c r="FT19" s="13"/>
+      <c r="FU19" s="13"/>
+      <c r="FV19" s="13"/>
+      <c r="FW19" s="13"/>
+      <c r="FX19" s="13"/>
+      <c r="FY19" s="13"/>
+      <c r="FZ19" s="13"/>
+      <c r="GA19" s="13"/>
+      <c r="GB19" s="13"/>
+      <c r="GC19" s="13"/>
+      <c r="GD19" s="13"/>
+      <c r="GE19" s="13"/>
+      <c r="GF19" s="13"/>
+      <c r="GG19" s="13"/>
+      <c r="GH19" s="13"/>
+      <c r="GI19" s="13"/>
+      <c r="GJ19" s="13"/>
+      <c r="GK19" s="13"/>
+      <c r="GL19" s="13"/>
+      <c r="GM19" s="13"/>
+      <c r="GN19" s="13"/>
+      <c r="GO19" s="13"/>
+      <c r="GP19" s="13"/>
+      <c r="GQ19" s="13"/>
+      <c r="GR19" s="13"/>
+      <c r="GS19" s="13"/>
+      <c r="GT19" s="13"/>
+      <c r="GU19" s="13"/>
+      <c r="GV19" s="13"/>
+      <c r="GW19" s="13"/>
+      <c r="GX19" s="13"/>
+      <c r="GY19" s="13"/>
+      <c r="GZ19" s="13"/>
+      <c r="HA19" s="13"/>
+      <c r="HB19" s="13"/>
+      <c r="HC19" s="13"/>
+      <c r="HD19" s="13"/>
+      <c r="HE19" s="13"/>
+      <c r="HF19" s="13"/>
+      <c r="HG19" s="13"/>
+      <c r="HH19" s="13"/>
+      <c r="HI19" s="13"/>
+      <c r="HJ19" s="13"/>
+      <c r="HK19" s="13"/>
+      <c r="HL19" s="13"/>
+      <c r="HM19" s="13"/>
+      <c r="HN19" s="13"/>
+      <c r="HO19" s="13"/>
+      <c r="HP19" s="13"/>
+      <c r="HQ19" s="13"/>
+      <c r="HR19" s="13"/>
+      <c r="HS19" s="13"/>
+      <c r="HT19" s="13"/>
+      <c r="HU19" s="13"/>
+      <c r="HV19" s="13"/>
+      <c r="HW19" s="13"/>
+      <c r="HX19" s="13"/>
+      <c r="HY19" s="13"/>
+      <c r="HZ19" s="13"/>
+      <c r="IA19" s="13"/>
+      <c r="IB19" s="13"/>
+      <c r="IC19" s="13"/>
+      <c r="ID19" s="13"/>
+      <c r="IE19" s="13"/>
+      <c r="IF19" s="13"/>
+      <c r="IG19" s="13"/>
+      <c r="IH19" s="13"/>
+      <c r="II19" s="13"/>
+      <c r="IJ19" s="13"/>
+      <c r="IK19" s="13"/>
+      <c r="IL19" s="13"/>
+      <c r="IM19" s="13"/>
+      <c r="IN19" s="13"/>
+      <c r="IO19" s="13"/>
+      <c r="IP19" s="13"/>
+      <c r="IQ19" s="13"/>
+      <c r="IR19" s="13"/>
+      <c r="IS19" s="13"/>
+      <c r="IT19" s="13"/>
+      <c r="IU19" s="13"/>
+      <c r="IV19" s="13"/>
+    </row>
+    <row r="20" spans="1:256" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:256" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="9">
+        <v>41820</v>
+      </c>
+      <c r="C21" s="9">
+        <v>41851</v>
+      </c>
+      <c r="D21" s="9">
+        <v>41882</v>
+      </c>
+      <c r="E21" s="9">
+        <v>41912</v>
+      </c>
+      <c r="F21" s="9">
+        <v>41943</v>
+      </c>
+      <c r="G21" s="9">
+        <v>41973</v>
+      </c>
+      <c r="H21" s="9">
+        <v>42004</v>
+      </c>
+      <c r="I21" s="9">
+        <v>42035</v>
+      </c>
+      <c r="J21" s="9">
+        <v>42063</v>
+      </c>
+      <c r="K21" s="9">
+        <v>42094</v>
+      </c>
+      <c r="L21" s="9">
+        <v>42124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:256" ht="48" customHeight="1" thickTop="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup scale="10" orientation="landscape"/>

</xml_diff>